<commit_message>
rm useles min 0 card e3166a45308d137308aaaa2c25e7a13ec004086e
</commit_message>
<xml_diff>
--- a/ig/nr-change-contained/StructureDefinition-pdsm-submissionset-comprehensive.xlsx
+++ b/ig/nr-change-contained/StructureDefinition-pdsm-submissionset-comprehensive.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-12T08:08:55+00:00</t>
+    <t>2023-07-12T08:12:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1004,10 +1004,10 @@
 </t>
   </si>
   <si>
-    <t>Organisation auteur du document</t>
-  </si>
-  <si>
-    <t>Un lot de soumission est obligatoirement associé à un auteur. Si l’attribut “source” n’est pas renseigné, autrement dit si l’auteur est une personne morale, la cardinalité est contrainte à [1..1].</t>
+    <t>Organisation auteur du document. Un lot de soumission est obligatoirement associé à un auteur. Si l’attribut “source” n’est pas renseigné, autrement dit si l’auteur est une personne morale, la cardinalité est contrainte à [1..1].</t>
+  </si>
+  <si>
+    <t>When the author of the SubmissionSet is an Organization, this extension shall be used.</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}

</xml_diff>